<commit_message>
better info in boxes
</commit_message>
<xml_diff>
--- a/MV2040 Indicators and Outcomes DRAFT baseline- August 2019.XLSX
+++ b/MV2040 Indicators and Outcomes DRAFT baseline- August 2019.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WilliamLa\Desktop\MV2040 outcomes framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1274E6-4C1B-41FE-96B7-A3C09CA45B9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A065B83F-6590-423B-B168-3BEDA017403B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22920" windowHeight="15240" activeTab="7" xr2:uid="{EDE946D3-B550-4852-B98C-D382147A5E7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22920" windowHeight="15240" activeTab="4" xr2:uid="{EDE946D3-B550-4852-B98C-D382147A5E7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Targets Indicators Measures" sheetId="9" r:id="rId1"/>
@@ -18400,8 +18400,8 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18481,7 +18481,7 @@
         <v>766</v>
       </c>
       <c r="K2" t="s">
-        <v>599</v>
+        <v>649</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -20555,7 +20555,7 @@
   </sheetPr>
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
function for ind theme text
</commit_message>
<xml_diff>
--- a/MV2040 Indicators and Outcomes DRAFT baseline- August 2019.XLSX
+++ b/MV2040 Indicators and Outcomes DRAFT baseline- August 2019.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WilliamLa\Desktop\MV2040 outcomes framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC75C03-3ED0-4CAB-B0C2-D2BEC2BCB760}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791986BD-2043-495F-997A-B7EC1BC427D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22920" windowHeight="15240" activeTab="2" xr2:uid="{EDE946D3-B550-4852-B98C-D382147A5E7C}"/>
   </bookViews>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2889" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2889" uniqueCount="619">
   <si>
     <t>FAIR</t>
   </si>
@@ -2077,6 +2077,9 @@
   </si>
   <si>
     <t>Based on the target in the Creating Liveable Cities in Australia document from RMIT.</t>
+  </si>
+  <si>
+    <t>Community Survey (baseline data from the 2011 VicHealth Indicators Survey)</t>
   </si>
 </sst>
 </file>
@@ -14454,7 +14457,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15990,7 +15993,7 @@
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4" t="s">
-        <v>73</v>
+        <v>618</v>
       </c>
       <c r="H41" s="43" t="s">
         <v>354</v>
@@ -16738,8 +16741,8 @@
   </sheetPr>
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69:B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17356,7 +17359,7 @@
         <v>448</v>
       </c>
       <c r="B36" s="63">
-        <v>40724</v>
+        <v>40764</v>
       </c>
       <c r="C36" s="68">
         <v>16.7</v>
@@ -17372,7 +17375,7 @@
         <v>448</v>
       </c>
       <c r="B37" s="63">
-        <v>42551</v>
+        <v>42591</v>
       </c>
       <c r="C37" s="68">
         <v>15.9</v>
@@ -17484,7 +17487,7 @@
         <v>451</v>
       </c>
       <c r="B44" s="63">
-        <v>40724</v>
+        <v>40764</v>
       </c>
       <c r="C44" s="68">
         <v>15.3</v>
@@ -17500,7 +17503,7 @@
         <v>451</v>
       </c>
       <c r="B45" s="63">
-        <v>42551</v>
+        <v>42591</v>
       </c>
       <c r="C45" s="68">
         <v>17.8</v>
@@ -17627,8 +17630,8 @@
       <c r="A53" s="32" t="s">
         <v>454</v>
       </c>
-      <c r="B53" s="65">
-        <v>40724</v>
+      <c r="B53" s="63">
+        <v>40764</v>
       </c>
       <c r="C53" s="68">
         <v>33.799999999999997</v>
@@ -17643,8 +17646,8 @@
       <c r="A54" s="32" t="s">
         <v>454</v>
       </c>
-      <c r="B54" s="65">
-        <v>42551</v>
+      <c r="B54" s="63">
+        <v>42591</v>
       </c>
       <c r="C54" s="68">
         <v>33</v>
@@ -17844,7 +17847,7 @@
         <v>459</v>
       </c>
       <c r="B66" s="63">
-        <v>40724</v>
+        <v>40764</v>
       </c>
       <c r="C66" s="68">
         <v>21.6</v>
@@ -17860,7 +17863,7 @@
         <v>459</v>
       </c>
       <c r="B67" s="63">
-        <v>42551</v>
+        <v>42591</v>
       </c>
       <c r="C67" s="68">
         <v>23.6</v>
@@ -17892,7 +17895,7 @@
         <v>460</v>
       </c>
       <c r="B69" s="63">
-        <v>40724</v>
+        <v>40764</v>
       </c>
       <c r="C69" s="68">
         <v>10.4</v>
@@ -17908,7 +17911,7 @@
         <v>460</v>
       </c>
       <c r="B70" s="63">
-        <v>42551</v>
+        <v>42591</v>
       </c>
       <c r="C70" s="68">
         <v>11</v>

</xml_diff>

<commit_message>
target added to theme graphs
</commit_message>
<xml_diff>
--- a/MV2040 Indicators and Outcomes DRAFT baseline- August 2019.XLSX
+++ b/MV2040 Indicators and Outcomes DRAFT baseline- August 2019.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WilliamLa\Desktop\MV2040 outcomes framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F962CEE6-6090-4C1D-96EE-719C5DD38255}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82CC9EE-4130-41E9-BF66-281A9D3AEEFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22920" windowHeight="15240" activeTab="6" xr2:uid="{EDE946D3-B550-4852-B98C-D382147A5E7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22920" windowHeight="15240" activeTab="2" xr2:uid="{EDE946D3-B550-4852-B98C-D382147A5E7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Targets Indicators Measures" sheetId="9" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2893" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2893" uniqueCount="620">
   <si>
     <t>FAIR</t>
   </si>
@@ -2080,6 +2080,9 @@
   </si>
   <si>
     <t>Index score</t>
+  </si>
+  <si>
+    <t>This is a statewide measure of library usage and allows for comapison with other municipalities.</t>
   </si>
 </sst>
 </file>
@@ -14459,8 +14462,8 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15072,8 +15075,8 @@
       <c r="I16" s="5" t="s">
         <v>526</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>510</v>
+      <c r="J16" s="5" t="s">
+        <v>619</v>
       </c>
       <c r="K16" t="s">
         <v>351</v>
@@ -18717,7 +18720,7 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated public transport calcs
</commit_message>
<xml_diff>
--- a/MV2040 Indicators and Outcomes DRAFT baseline- August 2019.XLSX
+++ b/MV2040 Indicators and Outcomes DRAFT baseline- August 2019.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WilliamLa\Desktop\MV2040 outcomes framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B5114F-4DBB-4493-A221-8D8E19102543}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C26386-37D9-443D-8258-A6BBC71242F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22920" windowHeight="15240" xr2:uid="{EDE946D3-B550-4852-B98C-D382147A5E7C}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="data_format" sheetId="15" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">data!$A$1:$F$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">data!$A$1:$F$124</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicator_list!$K$1:$K$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="361">
   <si>
     <t>FAIR</t>
   </si>
@@ -1105,9 +1105,6 @@
     <t xml:space="preserve">A well-integrated and accessible public transport system has potential to reduce traffic congestion in a city and improve residents' access to jobs and goods and services. Reducing reliance on private vehicle travel also has significant safety, health, social and environmental benefits. </t>
   </si>
   <si>
-    <t xml:space="preserve">This is an interim figure only!!!  --- Building new developments within a 400-800m walking distance is generally in line with the Transit Oriented Development (TOD) principles. Increasing density in activity centres, which are generally well serviced by public transport, is outlined in the Plan Melbourne strategy, which Council follows. As such, a significant number of new dwellings is and will continue to be built in activity centres. </t>
-  </si>
-  <si>
     <t>Contribute</t>
   </si>
   <si>
@@ -1137,6 +1134,12 @@
   </si>
   <si>
     <t xml:space="preserve">Poor mental health can be associated with reduced physical health and fitness, lower life expectancy and higher morbidity. Positive mental health and wellbeing help to build community resilience and encourage our community to be productive and contribute to our community. </t>
+  </si>
+  <si>
+    <t>Aspirational target for the majority of properties to have access to frequent public transport services.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Building new developments within a 400-800m walking distance is generally in line with the Transit Oriented Development (TOD) principles. Increasing density in activity centres, which are generally well serviced by public transport, is outlined in the Plan Melbourne strategy, which Council follows. As such, a significant number of new dwellings is and will continue to be built in activity centres. </t>
   </si>
 </sst>
 </file>
@@ -2153,8 +2156,8 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,13 +2234,13 @@
         <v>231</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J2" t="s">
         <v>133</v>
       </c>
       <c r="K2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L2" t="s">
         <v>283</v>
@@ -2269,13 +2272,13 @@
         <v>232</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J3" t="s">
         <v>109</v>
       </c>
       <c r="K3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L3" t="s">
         <v>283</v>
@@ -2307,13 +2310,13 @@
         <v>233</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J4" t="s">
         <v>109</v>
       </c>
       <c r="K4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L4" t="s">
         <v>283</v>
@@ -2345,7 +2348,7 @@
         <v>256</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J5" t="s">
         <v>109</v>
@@ -2383,13 +2386,13 @@
         <v>234</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J6" t="s">
         <v>109</v>
       </c>
       <c r="K6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L6" t="s">
         <v>283</v>
@@ -2421,13 +2424,13 @@
         <v>235</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J7" t="s">
         <v>109</v>
       </c>
       <c r="K7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L7" t="s">
         <v>283</v>
@@ -2459,13 +2462,13 @@
         <v>237</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J8" t="s">
         <v>133</v>
       </c>
       <c r="K8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L8" t="s">
         <v>283</v>
@@ -2497,13 +2500,13 @@
         <v>236</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J9" t="s">
         <v>109</v>
       </c>
       <c r="K9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L9" t="s">
         <v>283</v>
@@ -2541,7 +2544,7 @@
         <v>109</v>
       </c>
       <c r="K10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L10" t="s">
         <v>286</v>
@@ -2611,13 +2614,13 @@
         <v>238</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J12" t="s">
         <v>133</v>
       </c>
       <c r="K12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L12" t="s">
         <v>287</v>
@@ -2655,7 +2658,7 @@
         <v>133</v>
       </c>
       <c r="K13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L13" t="s">
         <v>281</v>
@@ -2693,7 +2696,7 @@
         <v>109</v>
       </c>
       <c r="K14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L14" t="s">
         <v>285</v>
@@ -2927,7 +2930,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>176</v>
       </c>
@@ -2947,10 +2950,10 @@
         <v>291</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>314</v>
-      </c>
-      <c r="H21" s="38" t="s">
-        <v>349</v>
+        <v>359</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>360</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>348</v>
@@ -2997,7 +3000,7 @@
         <v>109</v>
       </c>
       <c r="K22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L22" t="s">
         <v>279</v>
@@ -3035,7 +3038,7 @@
         <v>109</v>
       </c>
       <c r="K23" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L23" t="s">
         <v>279</v>
@@ -3073,7 +3076,7 @@
         <v>133</v>
       </c>
       <c r="K24" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L24" t="s">
         <v>279</v>
@@ -3453,7 +3456,7 @@
         <v>109</v>
       </c>
       <c r="K34" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L34" t="s">
         <v>275</v>
@@ -3491,7 +3494,7 @@
         <v>109</v>
       </c>
       <c r="K35" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L35" t="s">
         <v>275</v>
@@ -3529,7 +3532,7 @@
         <v>109</v>
       </c>
       <c r="K36" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L36" t="s">
         <v>275</v>
@@ -3719,7 +3722,7 @@
         <v>109</v>
       </c>
       <c r="K41" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L41" t="s">
         <v>276</v>
@@ -4454,10 +4457,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:H123"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="I100" sqref="I100"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="O69" sqref="O69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5607,10 +5610,10 @@
         <v>176</v>
       </c>
       <c r="B68" s="30">
-        <v>43281</v>
+        <v>43444</v>
       </c>
       <c r="C68" s="34">
-        <v>76.099999999999994</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="D68" s="26"/>
       <c r="E68" s="26"/>
@@ -5619,51 +5622,51 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="23" t="s">
+      <c r="A69" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="B69" s="29">
-        <v>51317</v>
+      <c r="B69" s="30">
+        <v>43780</v>
       </c>
       <c r="C69" s="34">
-        <v>90</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="D69" s="26"/>
       <c r="E69" s="26"/>
-      <c r="F69" s="1" t="s">
-        <v>204</v>
+      <c r="F69" s="7" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="35" t="s">
-        <v>177</v>
+      <c r="A70" s="23" t="s">
+        <v>176</v>
       </c>
       <c r="B70" s="29">
-        <v>40764</v>
+        <v>51317</v>
       </c>
       <c r="C70" s="34">
-        <v>21.6</v>
+        <v>90</v>
       </c>
       <c r="D70" s="26"/>
       <c r="E70" s="26"/>
-      <c r="F70" s="7" t="s">
-        <v>227</v>
+      <c r="F70" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="23" t="s">
+      <c r="A71" s="35" t="s">
         <v>177</v>
       </c>
       <c r="B71" s="29">
-        <v>42591</v>
+        <v>40764</v>
       </c>
       <c r="C71" s="34">
-        <v>23.6</v>
+        <v>21.6</v>
       </c>
       <c r="D71" s="26"/>
       <c r="E71" s="26"/>
       <c r="F71" s="7" t="s">
-        <v>202</v>
+        <v>227</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -5671,47 +5674,47 @@
         <v>177</v>
       </c>
       <c r="B72" s="29">
-        <v>51317</v>
+        <v>42591</v>
       </c>
       <c r="C72" s="34">
-        <v>50.1</v>
+        <v>23.6</v>
       </c>
       <c r="D72" s="26"/>
       <c r="E72" s="26"/>
-      <c r="F72" s="1" t="s">
-        <v>204</v>
+      <c r="F72" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="36" t="s">
-        <v>178</v>
+      <c r="A73" s="23" t="s">
+        <v>177</v>
       </c>
       <c r="B73" s="29">
-        <v>40764</v>
+        <v>51317</v>
       </c>
       <c r="C73" s="34">
-        <v>10.4</v>
+        <v>50.1</v>
       </c>
       <c r="D73" s="26"/>
       <c r="E73" s="26"/>
       <c r="F73" s="1" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="36" t="s">
         <v>178</v>
       </c>
       <c r="B74" s="29">
-        <v>42591</v>
+        <v>40764</v>
       </c>
       <c r="C74" s="34">
-        <v>11</v>
+        <v>10.4</v>
       </c>
       <c r="D74" s="26"/>
       <c r="E74" s="26"/>
-      <c r="F74" s="7" t="s">
-        <v>202</v>
+      <c r="F74" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -5719,31 +5722,31 @@
         <v>178</v>
       </c>
       <c r="B75" s="29">
-        <v>51317</v>
+        <v>42591</v>
       </c>
       <c r="C75" s="34">
-        <v>11.600000000000001</v>
+        <v>11</v>
       </c>
       <c r="D75" s="26"/>
       <c r="E75" s="26"/>
-      <c r="F75" s="1" t="s">
-        <v>204</v>
+      <c r="F75" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="37" t="s">
-        <v>179</v>
+      <c r="A76" s="23" t="s">
+        <v>178</v>
       </c>
       <c r="B76" s="29">
-        <v>42004</v>
+        <v>51317</v>
       </c>
       <c r="C76" s="34">
-        <v>68</v>
+        <v>11.600000000000001</v>
       </c>
       <c r="D76" s="26"/>
       <c r="E76" s="26"/>
       <c r="F76" s="1" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -5751,10 +5754,10 @@
         <v>179</v>
       </c>
       <c r="B77" s="29">
-        <v>42369</v>
+        <v>42004</v>
       </c>
       <c r="C77" s="34">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="D77" s="26"/>
       <c r="E77" s="26"/>
@@ -5767,10 +5770,10 @@
         <v>179</v>
       </c>
       <c r="B78" s="29">
-        <v>42735</v>
+        <v>42369</v>
       </c>
       <c r="C78" s="34">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D78" s="26"/>
       <c r="E78" s="26"/>
@@ -5783,10 +5786,10 @@
         <v>179</v>
       </c>
       <c r="B79" s="29">
-        <v>43100</v>
+        <v>42735</v>
       </c>
       <c r="C79" s="34">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="D79" s="26"/>
       <c r="E79" s="26"/>
@@ -5795,19 +5798,19 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="23" t="s">
+      <c r="A80" s="37" t="s">
         <v>179</v>
       </c>
       <c r="B80" s="29">
-        <v>43465</v>
-      </c>
-      <c r="C80" s="28">
-        <v>23</v>
-      </c>
-      <c r="D80" s="28"/>
-      <c r="E80" s="28"/>
-      <c r="F80" s="7" t="s">
-        <v>202</v>
+        <v>43100</v>
+      </c>
+      <c r="C80" s="34">
+        <v>22</v>
+      </c>
+      <c r="D80" s="26"/>
+      <c r="E80" s="26"/>
+      <c r="F80" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -5815,63 +5818,63 @@
         <v>179</v>
       </c>
       <c r="B81" s="29">
-        <v>51501</v>
+        <v>43465</v>
       </c>
       <c r="C81" s="28">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D81" s="28"/>
       <c r="E81" s="28"/>
-      <c r="F81" s="1" t="s">
-        <v>204</v>
+      <c r="F81" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="B82" s="30">
-        <v>43281</v>
-      </c>
-      <c r="C82" s="34">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="D82" s="26"/>
-      <c r="E82" s="26"/>
-      <c r="F82" s="7" t="s">
-        <v>202</v>
+        <v>179</v>
+      </c>
+      <c r="B82" s="29">
+        <v>51501</v>
+      </c>
+      <c r="C82" s="28">
+        <v>0</v>
+      </c>
+      <c r="D82" s="28"/>
+      <c r="E82" s="28"/>
+      <c r="F82" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="B83" s="29">
-        <v>51317</v>
+      <c r="B83" s="30">
+        <v>43281</v>
       </c>
       <c r="C83" s="34">
-        <v>100</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="D83" s="26"/>
       <c r="E83" s="26"/>
-      <c r="F83" s="1" t="s">
-        <v>204</v>
+      <c r="F83" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="B84" s="30">
-        <v>43281</v>
+        <v>180</v>
+      </c>
+      <c r="B84" s="29">
+        <v>51317</v>
       </c>
       <c r="C84" s="34">
-        <v>0</v>
-      </c>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="7" t="s">
-        <v>202</v>
+        <v>100</v>
+      </c>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -5879,47 +5882,47 @@
         <v>181</v>
       </c>
       <c r="B85" s="30">
-        <v>43646</v>
+        <v>43281</v>
       </c>
       <c r="C85" s="34">
-        <v>60.699999999999996</v>
+        <v>0</v>
       </c>
       <c r="D85" s="27"/>
       <c r="E85" s="27"/>
       <c r="F85" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="B86" s="29">
-        <v>51317</v>
+      <c r="B86" s="30">
+        <v>43646</v>
       </c>
       <c r="C86" s="34">
-        <v>100</v>
+        <v>60.699999999999996</v>
       </c>
       <c r="D86" s="27"/>
       <c r="E86" s="27"/>
-      <c r="F86" s="1" t="s">
+      <c r="F86" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B87" s="29">
+        <v>51317</v>
+      </c>
+      <c r="C87" s="34">
+        <v>100</v>
+      </c>
+      <c r="D87" s="27"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="1" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="B87" s="30">
-        <v>43281</v>
-      </c>
-      <c r="C87" s="28">
-        <v>2773</v>
-      </c>
-      <c r="D87" s="28"/>
-      <c r="E87" s="28"/>
-      <c r="F87" s="7" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -5927,79 +5930,79 @@
         <v>182</v>
       </c>
       <c r="B88" s="30">
-        <v>43646</v>
+        <v>43281</v>
       </c>
       <c r="C88" s="28">
-        <v>1746</v>
+        <v>2773</v>
       </c>
       <c r="D88" s="28"/>
       <c r="E88" s="28"/>
       <c r="F88" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="B89" s="29">
-        <v>51317</v>
+      <c r="B89" s="30">
+        <v>43646</v>
       </c>
       <c r="C89" s="28">
-        <v>139</v>
+        <v>1746</v>
       </c>
       <c r="D89" s="28"/>
       <c r="E89" s="28"/>
-      <c r="F89" s="1" t="s">
-        <v>204</v>
+      <c r="F89" s="7" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="B90" s="30">
-        <v>43281</v>
+        <v>182</v>
+      </c>
+      <c r="B90" s="29">
+        <v>51317</v>
       </c>
       <c r="C90" s="28">
-        <v>1300000</v>
+        <v>139</v>
       </c>
       <c r="D90" s="28"/>
       <c r="E90" s="28"/>
-      <c r="F90" s="7" t="s">
-        <v>202</v>
+      <c r="F90" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="B91" s="29">
-        <v>51317</v>
+      <c r="B91" s="30">
+        <v>43281</v>
       </c>
       <c r="C91" s="28">
-        <v>0</v>
+        <v>1300000</v>
       </c>
       <c r="D91" s="28"/>
       <c r="E91" s="28"/>
-      <c r="F91" s="1" t="s">
-        <v>204</v>
+      <c r="F91" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B92" s="30">
-        <v>43281</v>
+        <v>189</v>
+      </c>
+      <c r="B92" s="29">
+        <v>51317</v>
       </c>
       <c r="C92" s="28">
-        <v>49917</v>
+        <v>0</v>
       </c>
       <c r="D92" s="28"/>
       <c r="E92" s="28"/>
-      <c r="F92" s="7" t="s">
-        <v>202</v>
+      <c r="F92" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -6007,193 +6010,195 @@
         <v>183</v>
       </c>
       <c r="B93" s="30">
-        <v>43646</v>
+        <v>43281</v>
       </c>
       <c r="C93" s="28">
-        <v>51573</v>
+        <v>49917</v>
       </c>
       <c r="D93" s="28"/>
       <c r="E93" s="28"/>
       <c r="F93" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="B94" s="29">
-        <v>51317</v>
+      <c r="B94" s="30">
+        <v>43646</v>
       </c>
       <c r="C94" s="28">
-        <v>64892</v>
+        <v>51573</v>
       </c>
       <c r="D94" s="28"/>
       <c r="E94" s="28"/>
-      <c r="F94" s="1" t="s">
-        <v>204</v>
+      <c r="F94" s="7" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="B95" s="30">
-        <v>42185</v>
+        <v>183</v>
+      </c>
+      <c r="B95" s="29">
+        <v>51317</v>
       </c>
       <c r="C95" s="28">
-        <v>127</v>
+        <v>64892</v>
       </c>
       <c r="D95" s="28"/>
       <c r="E95" s="28"/>
-      <c r="F95" s="7" t="s">
-        <v>202</v>
+      <c r="F95" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="B96" s="29">
-        <v>51317</v>
+      <c r="B96" s="30">
+        <v>42185</v>
       </c>
       <c r="C96" s="28">
-        <v>57</v>
+        <v>127</v>
       </c>
       <c r="D96" s="28"/>
       <c r="E96" s="28"/>
-      <c r="F96" s="1" t="s">
-        <v>204</v>
+      <c r="F96" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="B97" s="30">
-        <v>42185</v>
+        <v>190</v>
+      </c>
+      <c r="B97" s="29">
+        <v>51317</v>
       </c>
       <c r="C97" s="28">
-        <v>12000</v>
+        <v>57</v>
       </c>
       <c r="D97" s="28"/>
       <c r="E97" s="28"/>
-      <c r="F97" s="7" t="s">
-        <v>202</v>
+      <c r="F97" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="B98" s="29">
-        <v>51317</v>
+      <c r="B98" s="30">
+        <v>42185</v>
       </c>
       <c r="C98" s="28">
-        <v>6700</v>
+        <v>12000</v>
       </c>
       <c r="D98" s="28"/>
       <c r="E98" s="28"/>
-      <c r="F98" s="1" t="s">
-        <v>204</v>
+      <c r="F98" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="B99" s="30">
-        <v>43281</v>
-      </c>
-      <c r="C99" s="34">
-        <v>17</v>
-      </c>
-      <c r="D99" s="34">
-        <v>16</v>
-      </c>
-      <c r="E99" s="34">
-        <v>18</v>
-      </c>
-      <c r="F99" s="7" t="s">
-        <v>202</v>
+        <v>191</v>
+      </c>
+      <c r="B99" s="29">
+        <v>51317</v>
+      </c>
+      <c r="C99" s="28">
+        <v>6700</v>
+      </c>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="B100" s="29">
-        <v>51317</v>
+      <c r="B100" s="30">
+        <v>43281</v>
       </c>
       <c r="C100" s="34">
-        <v>30</v>
-      </c>
-      <c r="D100" s="34"/>
-      <c r="E100" s="34"/>
-      <c r="F100" s="1" t="s">
-        <v>204</v>
+        <v>17</v>
+      </c>
+      <c r="D100" s="34">
+        <v>16</v>
+      </c>
+      <c r="E100" s="34">
+        <v>18</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="B101" s="30">
-        <v>42185</v>
+        <v>192</v>
+      </c>
+      <c r="B101" s="29">
+        <v>51317</v>
       </c>
       <c r="C101" s="34">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D101" s="34"/>
       <c r="E101" s="34"/>
-      <c r="F101" s="7" t="s">
-        <v>202</v>
+      <c r="F101" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="B102" s="29">
-        <v>51317</v>
+      <c r="B102" s="30">
+        <v>42185</v>
       </c>
       <c r="C102" s="34">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D102" s="34"/>
       <c r="E102" s="34"/>
-      <c r="F102" s="1" t="s">
-        <v>204</v>
+      <c r="F102" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B103" s="29">
         <v>51317</v>
       </c>
       <c r="C103" s="34">
-        <v>30</v>
-      </c>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
+        <v>35</v>
+      </c>
+      <c r="D103" s="34"/>
+      <c r="E103" s="34"/>
       <c r="F103" s="1" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="B104" s="30">
-        <v>43281</v>
+        <v>192</v>
+      </c>
+      <c r="B104" s="29">
+        <v>51317</v>
       </c>
       <c r="C104" s="34">
-        <v>41.67</v>
-      </c>
-      <c r="F104" s="7" t="s">
-        <v>202</v>
+        <v>30</v>
+      </c>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -6201,97 +6206,97 @@
         <v>184</v>
       </c>
       <c r="B105" s="30">
-        <v>43646</v>
+        <v>43281</v>
       </c>
       <c r="C105" s="34">
-        <v>41.11</v>
+        <v>41.67</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="B106" s="29">
-        <v>51317</v>
+      <c r="B106" s="30">
+        <v>43646</v>
       </c>
       <c r="C106" s="34">
-        <v>90</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>204</v>
+        <v>41.11</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="B107" s="30">
-        <v>43646</v>
+        <v>184</v>
+      </c>
+      <c r="B107" s="29">
+        <v>51317</v>
       </c>
       <c r="C107" s="34">
-        <v>50</v>
-      </c>
-      <c r="F107" s="7" t="s">
-        <v>202</v>
+        <v>90</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="B108" s="29">
-        <v>51317</v>
+      <c r="B108" s="30">
+        <v>43646</v>
       </c>
       <c r="C108" s="34">
-        <v>75</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>204</v>
+        <v>50</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="B109" s="30">
-        <v>43646</v>
+        <v>185</v>
+      </c>
+      <c r="B109" s="29">
+        <v>51317</v>
       </c>
       <c r="C109" s="34">
-        <v>80</v>
-      </c>
-      <c r="F109" s="7" t="s">
-        <v>202</v>
+        <v>75</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="B110" s="29">
+      <c r="B110" s="30">
+        <v>43646</v>
+      </c>
+      <c r="C110" s="34">
+        <v>80</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B111" s="29">
         <v>51317</v>
       </c>
-      <c r="C110" s="34">
+      <c r="C111" s="34">
         <v>100</v>
       </c>
-      <c r="F110" s="1" t="s">
+      <c r="F111" s="1" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="B111" s="30">
-        <v>43281</v>
-      </c>
-      <c r="C111" s="34">
-        <v>75</v>
-      </c>
-      <c r="F111" s="7" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -6299,41 +6304,41 @@
         <v>186</v>
       </c>
       <c r="B112" s="30">
-        <v>43646</v>
+        <v>43281</v>
       </c>
       <c r="C112" s="34">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="B113" s="29">
-        <v>51317</v>
+      <c r="B113" s="30">
+        <v>43646</v>
       </c>
       <c r="C113" s="34">
-        <v>100</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>204</v>
+        <v>80</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="B114" s="30">
-        <v>43281</v>
+        <v>186</v>
+      </c>
+      <c r="B114" s="29">
+        <v>51317</v>
       </c>
       <c r="C114" s="34">
-        <v>0</v>
-      </c>
-      <c r="F114" s="7" t="s">
-        <v>202</v>
+        <v>100</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -6341,41 +6346,41 @@
         <v>187</v>
       </c>
       <c r="B115" s="30">
-        <v>43646</v>
+        <v>43281</v>
       </c>
       <c r="C115" s="34">
-        <v>5.4</v>
+        <v>0</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B116" s="29">
-        <v>51317</v>
+      <c r="B116" s="30">
+        <v>43646</v>
       </c>
       <c r="C116" s="34">
-        <v>100</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>204</v>
+        <v>5.4</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="B117" s="30">
-        <v>43281</v>
-      </c>
-      <c r="C117" s="28">
-        <v>4.17</v>
-      </c>
-      <c r="F117" s="7" t="s">
-        <v>202</v>
+        <v>187</v>
+      </c>
+      <c r="B117" s="29">
+        <v>51317</v>
+      </c>
+      <c r="C117" s="34">
+        <v>100</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -6383,82 +6388,96 @@
         <v>195</v>
       </c>
       <c r="B118" s="30">
-        <v>43646</v>
+        <v>43281</v>
       </c>
       <c r="C118" s="28">
-        <v>4.13</v>
+        <v>4.17</v>
       </c>
       <c r="F118" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B119" s="29">
-        <v>51317</v>
+      <c r="B119" s="30">
+        <v>43646</v>
       </c>
       <c r="C119" s="28">
-        <v>4.38</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>204</v>
+        <v>4.13</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="B120" s="30">
-        <v>43281</v>
+        <v>195</v>
+      </c>
+      <c r="B120" s="29">
+        <v>51317</v>
       </c>
       <c r="C120" s="28">
-        <v>91.1</v>
-      </c>
-      <c r="F120" s="7" t="s">
-        <v>202</v>
+        <v>4.38</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="B121" s="29">
-        <v>51317</v>
-      </c>
-      <c r="C121">
-        <v>95</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>204</v>
+      <c r="B121" s="30">
+        <v>43281</v>
+      </c>
+      <c r="C121" s="28">
+        <v>91.1</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="B122" s="31">
-        <v>40724</v>
-      </c>
-      <c r="C122" s="34">
-        <v>55.000000000000007</v>
-      </c>
-      <c r="F122" s="7" t="s">
-        <v>202</v>
+        <v>188</v>
+      </c>
+      <c r="B122" s="29">
+        <v>51317</v>
+      </c>
+      <c r="C122">
+        <v>95</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="B123" s="29">
+      <c r="B123" s="31">
+        <v>40724</v>
+      </c>
+      <c r="C123" s="34">
+        <v>55.000000000000007</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B124" s="29">
         <v>51317</v>
       </c>
-      <c r="C123" s="34">
+      <c r="C124" s="34">
         <v>57.8</v>
       </c>
-      <c r="F123" s="1" t="s">
+      <c r="F124" s="1" t="s">
         <v>204</v>
       </c>
     </row>

</xml_diff>